<commit_message>
time update and debugging on GSOM
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>30/6/2013</t>
+  </si>
+  <si>
+    <t>13/7/2013</t>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,11 +644,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>18.283333333333335</v>
+        <v>19.933333333333334</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1279,24 +1282,48 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="11"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+      <c r="A61" s="10">
+        <v>41554</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="11"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+      <c r="A62" s="10">
+        <v>41585</v>
+      </c>
+      <c r="B62" s="1">
+        <v>2</v>
+      </c>
+      <c r="C62" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="A63" s="10">
+        <v>41615</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1">
+        <v>45</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="A64" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" s="1">
+        <v>5</v>
+      </c>
+      <c r="C64" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>

</xml_diff>

<commit_message>
time update and debugging the GSOM algorithm
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>13/7/2013</t>
+  </si>
+  <si>
+    <t>14/7/2013</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,11 +647,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>19.933333333333334</v>
+        <v>20.033333333333335</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1326,9 +1329,15 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="11"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="A65" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" s="1">
+        <v>2</v>
+      </c>
+      <c r="C65" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>

</xml_diff>

<commit_message>
time update and GSOM first phase complete.
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>15/7/2013</t>
+  </si>
+  <si>
+    <t>16/7/2013</t>
   </si>
 </sst>
 </file>
@@ -606,7 +609,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,11 +653,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>20.55</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1354,9 +1357,15 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
+      <c r="A67" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" s="1">
+        <v>5</v>
+      </c>
+      <c r="C67" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>

</xml_diff>

<commit_message>
time update and GSOM smoothing implementation complete
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>16/7/2013</t>
+  </si>
+  <si>
+    <t>17/7/2013</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,11 +656,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>20.7</v>
+        <v>21.033333333333335</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1368,9 +1371,15 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="A68" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" s="1">
+        <v>3</v>
+      </c>
+      <c r="C68" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>

</xml_diff>

<commit_message>
time update and GSOM code update
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>19/7/2013</t>
+  </si>
+  <si>
+    <t>20/7/2103</t>
+  </si>
+  <si>
+    <t>21/7/2013</t>
+  </si>
+  <si>
+    <t>22/7/2013</t>
   </si>
 </sst>
 </file>
@@ -617,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,11 +671,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>21.483333333333334</v>
+        <v>22.533333333333335</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1410,19 +1419,37 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="A71" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1</v>
+      </c>
+      <c r="C71" s="1">
+        <v>18</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="A72" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1</v>
+      </c>
+      <c r="C72" s="1">
+        <v>44</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="A73" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" s="1">
+        <v>5</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>

</xml_diff>

<commit_message>
time update and GSOM modifications
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -169,6 +169,27 @@
   </si>
   <si>
     <t>22/7/2013</t>
+  </si>
+  <si>
+    <t>23/7/2013</t>
+  </si>
+  <si>
+    <t>24/7/2013</t>
+  </si>
+  <si>
+    <t>25/7/2013</t>
+  </si>
+  <si>
+    <t>26/7/2013</t>
+  </si>
+  <si>
+    <t>27/7/2013</t>
+  </si>
+  <si>
+    <t>28/7/2013</t>
+  </si>
+  <si>
+    <t>29/7/2013</t>
   </si>
 </sst>
 </file>
@@ -627,7 +648,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,11 +692,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>22.533333333333335</v>
+        <v>23.033333333333335</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1452,39 +1473,81 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="A74" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
+      <c r="A75" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="A76" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1</v>
+      </c>
+      <c r="C76" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="A77" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="A78" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+      <c r="A79" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
+      <c r="A80" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B80" s="1">
+        <v>2</v>
+      </c>
+      <c r="C80" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>

</xml_diff>

<commit_message>
time update and graphical node representation beginning development
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,11 +698,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>23.316666666666666</v>
+        <v>24.083333333333332</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1578,9 +1578,15 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
+      <c r="A83" s="10">
+        <v>41282</v>
+      </c>
+      <c r="B83" s="1">
+        <v>3</v>
+      </c>
+      <c r="C83" s="1">
+        <v>46</v>
+      </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>

</xml_diff>

<commit_message>
time update & cleaning of data
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>13/8/2013</t>
+  </si>
+  <si>
+    <t>14/8/2013</t>
   </si>
 </sst>
 </file>
@@ -662,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +710,7 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
@@ -1730,9 +1733,15 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="11"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
+      <c r="A96" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B96" s="1">
+        <v>6</v>
+      </c>
+      <c r="C96" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="11"/>

</xml_diff>

<commit_message>
time update, Sammons projections and java doc files
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>18/8/2013</t>
+  </si>
+  <si>
+    <t>19/8/2013</t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,11 +725,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>29.65</v>
+        <v>30.233333333333334</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,13 +1795,23 @@
       <c r="A100" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
+      <c r="B100" s="1">
+        <v>5</v>
+      </c>
+      <c r="C100" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="11"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
+      <c r="A101" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B101" s="1">
+        <v>3</v>
+      </c>
+      <c r="C101" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="11"/>

</xml_diff>

<commit_message>
time update and Sammon's projection modifications
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>20/8/2013</t>
+  </si>
+  <si>
+    <t>21/8/2013</t>
   </si>
 </sst>
 </file>
@@ -684,7 +687,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,11 +731,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>30.733333333333334</v>
+        <v>31.65</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1828,9 +1831,15 @@
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="11"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
+      <c r="A103" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B103" s="1">
+        <v>3</v>
+      </c>
+      <c r="C103" s="1">
+        <v>55</v>
+      </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="11"/>

</xml_diff>

<commit_message>
time update and sammons projection update
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>21/8/2013</t>
+  </si>
+  <si>
+    <t>22/8/2013</t>
   </si>
 </sst>
 </file>
@@ -687,7 +690,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="I104" sqref="I104"/>
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,11 +734,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>31.233333333333334</v>
+        <v>31.816666666666666</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1842,9 +1845,15 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="11"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
+      <c r="A104" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B104" s="1">
+        <v>5</v>
+      </c>
+      <c r="C104" s="1">
+        <v>35</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="11"/>

</xml_diff>

<commit_message>
time update and Sammon 3D
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>22/8/2013</t>
+  </si>
+  <si>
+    <t>23/8/2013</t>
   </si>
 </sst>
 </file>
@@ -690,7 +693,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,11 +737,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>31.816666666666666</v>
+        <v>32.333333333333336</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1856,9 +1859,15 @@
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="11"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
+      <c r="A105" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B105" s="1">
+        <v>6</v>
+      </c>
+      <c r="C105" s="1">
+        <v>31</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="11"/>

</xml_diff>

<commit_message>
time update and sammons modifications
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>23/8/2013</t>
+  </si>
+  <si>
+    <t>24/8/2013</t>
+  </si>
+  <si>
+    <t>25/8/2013</t>
+  </si>
+  <si>
+    <t>26/8/2013</t>
   </si>
 </sst>
 </file>
@@ -693,7 +702,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,11 +746,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>32.333333333333336</v>
+        <v>32.950000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1870,19 +1879,37 @@
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="11"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
+      <c r="A106" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0</v>
+      </c>
+      <c r="C106" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="11"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
+      <c r="A107" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B107" s="1">
+        <v>4</v>
+      </c>
+      <c r="C107" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="11"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
+      <c r="A108" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B108" s="1">
+        <v>6</v>
+      </c>
+      <c r="C108" s="1">
+        <v>22</v>
+      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="11"/>

</xml_diff>

<commit_message>
time update and coding
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -705,7 +705,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+      <selection activeCell="H113" sqref="H113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,11 +749,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>33.133333333333333</v>
+        <v>32.833333333333336</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1919,10 +1919,10 @@
         <v>75</v>
       </c>
       <c r="B109" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C109" s="1">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
time update and progress report zero add
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>27/8/2013</t>
+  </si>
+  <si>
+    <t>28/8/2013</t>
   </si>
 </sst>
 </file>
@@ -705,7 +708,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H113" sqref="H113"/>
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,11 +752,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>32.833333333333336</v>
+        <v>33.166666666666664</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1926,9 +1929,15 @@
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="11"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
+      <c r="A110" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B110" s="1">
+        <v>7</v>
+      </c>
+      <c r="C110" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="11"/>

</xml_diff>

<commit_message>
time update / new project implementation for statistical data
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="G115" sqref="G115"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,11 +761,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>35.133333333333333</v>
+        <v>34.633333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2041,10 +2041,10 @@
         <v>41434</v>
       </c>
       <c r="B119" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C119" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
code implementation & time keeping
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -717,7 +717,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,11 +761,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>34.633333333333333</v>
+        <v>34.716666666666669</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2048,9 +2048,15 @@
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="11"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
+      <c r="A120" s="10">
+        <v>41464</v>
+      </c>
+      <c r="B120" s="1">
+        <v>3</v>
+      </c>
+      <c r="C120" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="11"/>

</xml_diff>

<commit_message>
time update and code update
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>13/9/2013</t>
+  </si>
+  <si>
+    <t>14/9/2013</t>
   </si>
 </sst>
 </file>
@@ -723,7 +726,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,11 +770,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>36.883333333333333</v>
+        <v>37.466666666666669</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2134,9 +2137,15 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="11"/>
-      <c r="B127" s="1"/>
-      <c r="C127" s="1"/>
+      <c r="A127" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B127" s="1">
+        <v>3</v>
+      </c>
+      <c r="C127" s="1">
+        <v>35</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="11"/>

</xml_diff>

<commit_message>
time update and dataset cleaning
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -265,6 +265,18 @@
   </si>
   <si>
     <t>14/9/2013</t>
+  </si>
+  <si>
+    <t>15/9/2013</t>
+  </si>
+  <si>
+    <t>16/9/2013</t>
+  </si>
+  <si>
+    <t>17/9/2013</t>
+  </si>
+  <si>
+    <t>18/9/2013</t>
   </si>
 </sst>
 </file>
@@ -726,7 +738,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F127" sqref="F127"/>
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,11 +782,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>37.799999999999997</v>
+        <v>38.299999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2148,24 +2160,48 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="11"/>
-      <c r="B128" s="1"/>
-      <c r="C128" s="1"/>
+      <c r="A128" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B128" s="1">
+        <v>0</v>
+      </c>
+      <c r="C128" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="11"/>
-      <c r="B129" s="1"/>
-      <c r="C129" s="1"/>
+      <c r="A129" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B129" s="1">
+        <v>0</v>
+      </c>
+      <c r="C129" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="11"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
+      <c r="A130" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B130" s="1">
+        <v>4</v>
+      </c>
+      <c r="C130" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="11"/>
-      <c r="B131" s="1"/>
-      <c r="C131" s="1"/>
+      <c r="A131" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B131" s="1">
+        <v>3</v>
+      </c>
+      <c r="C131" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="11"/>

</xml_diff>

<commit_message>
TIME UPDATE AND MEETING RECORDING
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Date</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>18/9/2013</t>
+  </si>
+  <si>
+    <t>19/9/2013</t>
+  </si>
+  <si>
+    <t>20/9/2013</t>
   </si>
 </sst>
 </file>
@@ -738,7 +744,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+      <selection activeCell="G134" sqref="G134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,11 +788,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>38.299999999999997</v>
+        <v>38.383333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2197,21 +2203,33 @@
         <v>86</v>
       </c>
       <c r="B131" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C131" s="1">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="11"/>
-      <c r="B132" s="1"/>
-      <c r="C132" s="1"/>
+      <c r="A132" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B132" s="1">
+        <v>2</v>
+      </c>
+      <c r="C132" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="11"/>
-      <c r="B133" s="1"/>
-      <c r="C133" s="1"/>
+      <c r="A133" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B133" s="1">
+        <v>9</v>
+      </c>
+      <c r="C133" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="11"/>

</xml_diff>

<commit_message>
time update and new probability project and the SCBW player data
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>21/9/2013</t>
+  </si>
+  <si>
+    <t>22/9/2013</t>
   </si>
 </sst>
 </file>
@@ -747,7 +750,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="E133" sqref="E133"/>
+      <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +794,7 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
@@ -2246,9 +2249,15 @@
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="11"/>
-      <c r="B135" s="1"/>
-      <c r="C135" s="1"/>
+      <c r="A135" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B135" s="1">
+        <v>7</v>
+      </c>
+      <c r="C135" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="11"/>

</xml_diff>

<commit_message>
time update BW data clean
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>22/9/2013</t>
+  </si>
+  <si>
+    <t>23/9/2013</t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
       <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
@@ -794,11 +797,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>39.133333333333333</v>
+        <v>39.633333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2260,9 +2263,15 @@
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="11"/>
-      <c r="B136" s="1"/>
-      <c r="C136" s="1"/>
+      <c r="A136" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B136" s="1">
+        <v>6</v>
+      </c>
+      <c r="C136" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="11"/>

</xml_diff>

<commit_message>
time update and weighted covariance code
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>26/9/2013</t>
+  </si>
+  <si>
+    <t>27/9/2013</t>
   </si>
 </sst>
 </file>
@@ -761,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,11 +809,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>41.966666666666669</v>
+        <v>42.25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2316,9 +2319,15 @@
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="11"/>
-      <c r="B140" s="1"/>
-      <c r="C140" s="1"/>
+      <c r="A140" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B140" s="1">
+        <v>8</v>
+      </c>
+      <c r="C140" s="1">
+        <v>17</v>
+      </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="11"/>

</xml_diff>

<commit_message>
time update, weighted covariance bug fix
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>27/9/2013</t>
+  </si>
+  <si>
+    <t>28/9/2013</t>
   </si>
 </sst>
 </file>
@@ -765,7 +768,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +812,7 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
@@ -2330,9 +2333,15 @@
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="11"/>
-      <c r="B141" s="1"/>
-      <c r="C141" s="1"/>
+      <c r="A141" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B141" s="1">
+        <v>9</v>
+      </c>
+      <c r="C141" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="11"/>

</xml_diff>

<commit_message>
time update and sequence modeling project.
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -777,7 +777,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="E154" sqref="E154"/>
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
@@ -2455,9 +2455,15 @@
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="11"/>
-      <c r="B151" s="1"/>
-      <c r="C151" s="1"/>
+      <c r="A151" s="10">
+        <v>41496</v>
+      </c>
+      <c r="B151" s="1">
+        <v>5</v>
+      </c>
+      <c r="C151" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="11"/>

</xml_diff>

<commit_message>
time update and program update on sequences
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -777,7 +777,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152"/>
+      <selection activeCell="G150" sqref="G150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,11 +821,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>44.1</v>
+        <v>44.8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2466,9 +2466,15 @@
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="11"/>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
+      <c r="A152" s="10">
+        <v>41527</v>
+      </c>
+      <c r="B152" s="1">
+        <v>5</v>
+      </c>
+      <c r="C152" s="1">
+        <v>42</v>
+      </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="11"/>

</xml_diff>

<commit_message>
time update and SOM coding
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -777,7 +777,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="G150" sqref="G150"/>
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,11 +821,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>44.8</v>
+        <v>45.31666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2477,9 +2477,15 @@
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="11"/>
-      <c r="B153" s="1"/>
-      <c r="C153" s="1"/>
+      <c r="A153" s="10">
+        <v>41557</v>
+      </c>
+      <c r="B153" s="1">
+        <v>2</v>
+      </c>
+      <c r="C153" s="1">
+        <v>31</v>
+      </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="11"/>

</xml_diff>

<commit_message>
time update, matlab bug fix, sequence model development
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C154" sqref="C154"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="I156" sqref="I156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,11 +821,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>493</v>
+        <v>501</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>45.31666666666667</v>
+        <v>45.833333333333336</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2481,16 +2481,22 @@
         <v>41557</v>
       </c>
       <c r="B153" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C153" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="11"/>
-      <c r="B154" s="1"/>
-      <c r="C154" s="1"/>
+      <c r="A154" s="10">
+        <v>41588</v>
+      </c>
+      <c r="B154" s="1">
+        <v>7</v>
+      </c>
+      <c r="C154" s="1">
+        <v>31</v>
+      </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="11"/>

</xml_diff>

<commit_message>
time update and sequence code
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="I156" sqref="I156"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
@@ -2499,9 +2499,15 @@
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="11"/>
-      <c r="B155" s="1"/>
-      <c r="C155" s="1"/>
+      <c r="A155" s="10">
+        <v>41618</v>
+      </c>
+      <c r="B155" s="1">
+        <v>4</v>
+      </c>
+      <c r="C155" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="11"/>

</xml_diff>

<commit_message>
time update and analysis prerequisites
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>13/10/2013</t>
+  </si>
+  <si>
+    <t>14/10/2013</t>
   </si>
 </sst>
 </file>
@@ -780,7 +783,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="K154" sqref="K154"/>
+      <selection activeCell="F158" sqref="F158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,11 +827,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>45.9</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2524,9 +2527,15 @@
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="11"/>
-      <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
+      <c r="A157" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B157" s="1">
+        <v>6</v>
+      </c>
+      <c r="C157" s="1">
+        <v>54</v>
+      </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="11"/>

</xml_diff>

<commit_message>
time update, meeting minutes
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>templar park</t>
+  </si>
+  <si>
+    <t>17/10/2013</t>
   </si>
 </sst>
 </file>
@@ -792,7 +795,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+      <selection activeCell="H163" sqref="H163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +844,7 @@
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>47.56666666666667</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2573,9 +2576,15 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="11"/>
-      <c r="B160" s="1"/>
-      <c r="C160" s="1"/>
+      <c r="A160" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B160" s="1">
+        <v>0</v>
+      </c>
+      <c r="C160" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="11"/>

</xml_diff>

<commit_message>
time update and sequence commit
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -840,7 +840,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
@@ -2800,9 +2800,15 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="11"/>
-      <c r="B176" s="1"/>
-      <c r="C176" s="1"/>
+      <c r="A176" s="10">
+        <v>41316</v>
+      </c>
+      <c r="B176" s="1">
+        <v>5</v>
+      </c>
+      <c r="C176" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="11"/>

</xml_diff>

<commit_message>
time update and FSM creation
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Date</t>
   </si>
@@ -379,14 +379,25 @@
   </si>
   <si>
     <t>MUPA dinner</t>
+  </si>
+  <si>
+    <t>Borobudur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -420,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -501,11 +512,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -534,6 +554,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -839,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122:C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,11 +914,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>54.883333333333333</v>
+        <v>55.05</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2194,13 +2223,13 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="10">
+      <c r="A122" s="15">
         <v>41526</v>
       </c>
-      <c r="B122" s="1">
-        <v>0</v>
-      </c>
-      <c r="C122" s="1">
+      <c r="B122" s="8">
+        <v>0</v>
+      </c>
+      <c r="C122" s="8">
         <v>0</v>
       </c>
       <c r="D122" t="s">
@@ -2442,68 +2471,68 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="10">
+      <c r="A144" s="15">
         <v>41284</v>
       </c>
-      <c r="B144" s="1">
-        <v>0</v>
-      </c>
-      <c r="C144" s="1">
+      <c r="B144" s="8">
+        <v>0</v>
+      </c>
+      <c r="C144" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="10">
+      <c r="A145" s="15">
         <v>41315</v>
       </c>
-      <c r="B145" s="1">
-        <v>0</v>
-      </c>
-      <c r="C145" s="1">
+      <c r="B145" s="8">
+        <v>0</v>
+      </c>
+      <c r="C145" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="10">
+      <c r="A146" s="15">
         <v>41343</v>
       </c>
-      <c r="B146" s="1">
-        <v>0</v>
-      </c>
-      <c r="C146" s="1">
+      <c r="B146" s="8">
+        <v>0</v>
+      </c>
+      <c r="C146" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="10">
+      <c r="A147" s="15">
         <v>41374</v>
       </c>
-      <c r="B147" s="1">
-        <v>0</v>
-      </c>
-      <c r="C147" s="1">
+      <c r="B147" s="8">
+        <v>0</v>
+      </c>
+      <c r="C147" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="10">
+      <c r="A148" s="15">
         <v>41404</v>
       </c>
-      <c r="B148" s="1">
-        <v>0</v>
-      </c>
-      <c r="C148" s="1">
+      <c r="B148" s="8">
+        <v>0</v>
+      </c>
+      <c r="C148" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="10">
+      <c r="A149" s="15">
         <v>41435</v>
       </c>
-      <c r="B149" s="1">
-        <v>0</v>
-      </c>
-      <c r="C149" s="1">
+      <c r="B149" s="8">
+        <v>0</v>
+      </c>
+      <c r="C149" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2596,13 +2625,13 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="11" t="s">
+      <c r="A158" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B158" s="1">
-        <v>0</v>
-      </c>
-      <c r="C158" s="1">
+      <c r="B158" s="8">
+        <v>0</v>
+      </c>
+      <c r="C158" s="8">
         <v>0</v>
       </c>
       <c r="D158" t="s">
@@ -2775,13 +2804,13 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="11" t="s">
+      <c r="A174" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B174" s="1">
-        <v>0</v>
-      </c>
-      <c r="C174" s="1">
+      <c r="B174" s="8">
+        <v>0</v>
+      </c>
+      <c r="C174" s="8">
         <v>0</v>
       </c>
       <c r="D174" t="s">
@@ -2810,82 +2839,117 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="11"/>
-      <c r="B177" s="1"/>
-      <c r="C177" s="1"/>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="11"/>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="10">
+        <v>41344</v>
+      </c>
+      <c r="B177" s="1">
+        <v>5</v>
+      </c>
+      <c r="C177" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="10">
+        <v>41375</v>
+      </c>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" s="11"/>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="10">
+        <v>41405</v>
+      </c>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="11"/>
-      <c r="B180" s="1"/>
-      <c r="C180" s="1"/>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="11"/>
-      <c r="B181" s="1"/>
-      <c r="C181" s="1"/>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="11"/>
-      <c r="B182" s="1"/>
-      <c r="C182" s="1"/>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="11"/>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="15">
+        <v>41436</v>
+      </c>
+      <c r="B180" s="8">
+        <v>0</v>
+      </c>
+      <c r="C180" s="8">
+        <v>0</v>
+      </c>
+      <c r="D180" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="15">
+        <v>41466</v>
+      </c>
+      <c r="B181" s="8">
+        <v>0</v>
+      </c>
+      <c r="C181" s="8">
+        <v>0</v>
+      </c>
+      <c r="D181" s="14"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="15">
+        <v>41497</v>
+      </c>
+      <c r="B182" s="8">
+        <v>0</v>
+      </c>
+      <c r="C182" s="8">
+        <v>0</v>
+      </c>
+      <c r="D182" s="14"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="10">
+        <v>41528</v>
+      </c>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="11"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="11"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="11"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="11"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="11"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="11"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="11"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="11"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="11"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3256,6 +3320,9 @@
       <c r="C265" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D180:D182"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
time update & sequence debugging
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -556,14 +556,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,7 +869,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122:C122"/>
+      <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,11 +914,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>580</v>
+        <v>586</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>55.05</v>
+        <v>55.366666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2223,7 +2223,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="15">
+      <c r="A122" s="14">
         <v>41526</v>
       </c>
       <c r="B122" s="8">
@@ -2471,7 +2471,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="15">
+      <c r="A144" s="14">
         <v>41284</v>
       </c>
       <c r="B144" s="8">
@@ -2482,7 +2482,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="15">
+      <c r="A145" s="14">
         <v>41315</v>
       </c>
       <c r="B145" s="8">
@@ -2493,7 +2493,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="15">
+      <c r="A146" s="14">
         <v>41343</v>
       </c>
       <c r="B146" s="8">
@@ -2504,7 +2504,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="15">
+      <c r="A147" s="14">
         <v>41374</v>
       </c>
       <c r="B147" s="8">
@@ -2515,7 +2515,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="15">
+      <c r="A148" s="14">
         <v>41404</v>
       </c>
       <c r="B148" s="8">
@@ -2526,7 +2526,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="15">
+      <c r="A149" s="14">
         <v>41435</v>
       </c>
       <c r="B149" s="8">
@@ -2625,7 +2625,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="16" t="s">
+      <c r="A158" s="15" t="s">
         <v>102</v>
       </c>
       <c r="B158" s="8">
@@ -2804,7 +2804,7 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="16" t="s">
+      <c r="A174" s="15" t="s">
         <v>119</v>
       </c>
       <c r="B174" s="8">
@@ -2854,8 +2854,12 @@
       <c r="A178" s="10">
         <v>41375</v>
       </c>
-      <c r="B178" s="1"/>
-      <c r="C178" s="1"/>
+      <c r="B178" s="1">
+        <v>6</v>
+      </c>
+      <c r="C178" s="1">
+        <v>19</v>
+      </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="10">
@@ -2865,7 +2869,7 @@
       <c r="C179" s="1"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="15">
+      <c r="A180" s="14">
         <v>41436</v>
       </c>
       <c r="B180" s="8">
@@ -2874,12 +2878,12 @@
       <c r="C180" s="8">
         <v>0</v>
       </c>
-      <c r="D180" s="14" t="s">
+      <c r="D180" s="16" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="15">
+      <c r="A181" s="14">
         <v>41466</v>
       </c>
       <c r="B181" s="8">
@@ -2888,10 +2892,10 @@
       <c r="C181" s="8">
         <v>0</v>
       </c>
-      <c r="D181" s="14"/>
+      <c r="D181" s="16"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="15">
+      <c r="A182" s="14">
         <v>41497</v>
       </c>
       <c r="B182" s="8">
@@ -2900,7 +2904,7 @@
       <c r="C182" s="8">
         <v>0</v>
       </c>
-      <c r="D182" s="14"/>
+      <c r="D182" s="16"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="10">

</xml_diff>

<commit_message>
time update and bug fix comments
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -869,7 +869,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+      <selection activeCell="I182" sqref="I182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,11 +914,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>55.366666666666667</v>
+        <v>55.783333333333331</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2865,8 +2865,12 @@
       <c r="A179" s="10">
         <v>41405</v>
       </c>
-      <c r="B179" s="1"/>
-      <c r="C179" s="1"/>
+      <c r="B179" s="1">
+        <v>0</v>
+      </c>
+      <c r="C179" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="14">
@@ -2910,8 +2914,12 @@
       <c r="A183" s="10">
         <v>41528</v>
       </c>
-      <c r="B183" s="1"/>
-      <c r="C183" s="1"/>
+      <c r="B183" s="1">
+        <v>3</v>
+      </c>
+      <c r="C183" s="1">
+        <v>25</v>
+      </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="11"/>

</xml_diff>

<commit_message>
time update and sequence modeling
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -869,7 +869,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="I182" sqref="I182"/>
+      <selection activeCell="A184" sqref="A184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,11 +914,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>55.783333333333331</v>
+        <v>56.4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2922,9 +2922,15 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="11"/>
-      <c r="B184" s="1"/>
-      <c r="C184" s="1"/>
+      <c r="A184" s="10">
+        <v>41558</v>
+      </c>
+      <c r="B184" s="1">
+        <v>3</v>
+      </c>
+      <c r="C184" s="1">
+        <v>37</v>
+      </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="11"/>

</xml_diff>

<commit_message>
time update, basic coding fixes and cosine similarity
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -869,7 +869,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="A184" sqref="A184"/>
+      <selection activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,11 +914,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>56.4</v>
+        <v>56.633333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2933,9 +2933,15 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="11"/>
-      <c r="B185" s="1"/>
-      <c r="C185" s="1"/>
+      <c r="A185" s="10">
+        <v>41589</v>
+      </c>
+      <c r="B185" s="1">
+        <v>6</v>
+      </c>
+      <c r="C185" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="11"/>

</xml_diff>

<commit_message>
time update & bug fixing
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>Date</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>17/11/2013</t>
+  </si>
+  <si>
+    <t>18/11/2013</t>
+  </si>
+  <si>
+    <t>19/11/2013</t>
   </si>
 </sst>
 </file>
@@ -884,7 +890,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+      <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,11 +935,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>624</v>
+        <v>640</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>58.25</v>
+        <v>58.85</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3025,14 +3031,26 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="11"/>
-      <c r="B192" s="1"/>
-      <c r="C192" s="1"/>
+      <c r="A192" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B192" s="1">
+        <v>15</v>
+      </c>
+      <c r="C192" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="11"/>
-      <c r="B193" s="1"/>
-      <c r="C193" s="1"/>
+      <c r="A193" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B193" s="1">
+        <v>1</v>
+      </c>
+      <c r="C193" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="11"/>

</xml_diff>

<commit_message>
new data files, results files and modified code to entertain the repeated winner issue
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>Date</t>
   </si>
@@ -421,6 +421,15 @@
   </si>
   <si>
     <t>24/11/2013</t>
+  </si>
+  <si>
+    <t>25/11/2013</t>
+  </si>
+  <si>
+    <t>Stagnate</t>
+  </si>
+  <si>
+    <t>26/11/2013</t>
   </si>
 </sst>
 </file>
@@ -909,7 +918,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="C199" sqref="C199"/>
+      <selection activeCell="F200" sqref="F200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +963,7 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
@@ -3130,14 +3139,29 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="11"/>
-      <c r="B199" s="1"/>
-      <c r="C199" s="1"/>
+      <c r="A199" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B199" s="1">
+        <v>0</v>
+      </c>
+      <c r="C199" s="1">
+        <v>0</v>
+      </c>
+      <c r="D199" s="16" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="11"/>
-      <c r="B200" s="1"/>
-      <c r="C200" s="1"/>
+      <c r="A200" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B200" s="1">
+        <v>3</v>
+      </c>
+      <c r="C200" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="11"/>

</xml_diff>

<commit_message>
time update, data files and code modifications.
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>Date</t>
   </si>
@@ -430,6 +430,12 @@
   </si>
   <si>
     <t>26/11/2013</t>
+  </si>
+  <si>
+    <t>27/11/2013</t>
+  </si>
+  <si>
+    <t>28/11/2013</t>
   </si>
 </sst>
 </file>
@@ -918,7 +924,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="F200" sqref="F200"/>
+      <selection activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,11 +969,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>666</v>
+        <v>676</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>60.95</v>
+        <v>61.6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3164,14 +3170,26 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="11"/>
-      <c r="B201" s="1"/>
-      <c r="C201" s="1"/>
+      <c r="A201" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B201" s="1">
+        <v>4</v>
+      </c>
+      <c r="C201" s="1">
+        <v>17</v>
+      </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="11"/>
-      <c r="B202" s="1"/>
-      <c r="C202" s="1"/>
+      <c r="A202" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B202" s="1">
+        <v>6</v>
+      </c>
+      <c r="C202" s="1">
+        <v>22</v>
+      </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="11"/>

</xml_diff>

<commit_message>
time update and threshold setting
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t>Date</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>28/11/2013</t>
+  </si>
+  <si>
+    <t>29/11/2013</t>
   </si>
 </sst>
 </file>
@@ -924,7 +927,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="C203" sqref="C203"/>
+      <selection activeCell="F213" sqref="F213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,11 +972,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>676</v>
+        <v>685</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>61.6</v>
+        <v>61.866666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3192,9 +3195,15 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="11"/>
-      <c r="B203" s="1"/>
-      <c r="C203" s="1"/>
+      <c r="A203" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B203" s="1">
+        <v>9</v>
+      </c>
+      <c r="C203" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="11"/>

</xml_diff>

<commit_message>
protein data, time update, code update
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="G205" sqref="G205"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="C209" sqref="C209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,11 +1051,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>691</v>
+        <v>696</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>62.466666666666669</v>
+        <v>62.68333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3324,8 +3324,12 @@
       <c r="A207" s="10">
         <v>41345</v>
       </c>
-      <c r="B207" s="1"/>
-      <c r="C207" s="1"/>
+      <c r="B207" s="1">
+        <v>0</v>
+      </c>
+      <c r="C207" s="1">
+        <v>0</v>
+      </c>
       <c r="D207" s="16" t="s">
         <v>162</v>
       </c>
@@ -3334,8 +3338,12 @@
       <c r="A208" s="10">
         <v>41376</v>
       </c>
-      <c r="B208" s="1"/>
-      <c r="C208" s="1"/>
+      <c r="B208" s="1">
+        <v>5</v>
+      </c>
+      <c r="C208" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="10">

</xml_diff>

<commit_message>
java code, time update, and u matrix
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="C211" sqref="C211"/>
+      <selection activeCell="E214" sqref="E214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,11 +1051,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>63.966666666666669</v>
+        <v>64.36666666666666</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3371,15 +3371,23 @@
       <c r="A211" s="10">
         <v>41467</v>
       </c>
-      <c r="B211" s="1"/>
-      <c r="C211" s="1"/>
+      <c r="B211" s="1">
+        <v>1</v>
+      </c>
+      <c r="C211" s="1">
+        <v>24</v>
+      </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="10">
         <v>41498</v>
       </c>
-      <c r="B212" s="1"/>
-      <c r="C212" s="1"/>
+      <c r="B212" s="1">
+        <v>1</v>
+      </c>
+      <c r="C212" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="17">

</xml_diff>

<commit_message>
time update and mtDNA
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="C253" sqref="C253"/>
+      <selection activeCell="B251" activeCellId="2" sqref="C251 B251 B251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,11 +1063,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>68.466666666666669</v>
+        <v>68.13333333333334</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3760,10 +3760,10 @@
         <v>166</v>
       </c>
       <c r="B251" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C251" s="1">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
time update & data bug fix
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="173">
   <si>
     <t>Date</t>
   </si>
@@ -517,6 +517,24 @@
   </si>
   <si>
     <t>16/1/2013</t>
+  </si>
+  <si>
+    <t>17/1/2013</t>
+  </si>
+  <si>
+    <t>18/1/2013</t>
+  </si>
+  <si>
+    <t>19/1/2013</t>
+  </si>
+  <si>
+    <t>20/1/2013</t>
+  </si>
+  <si>
+    <t>21/1/2013</t>
+  </si>
+  <si>
+    <t>Ankor Wat</t>
   </si>
 </sst>
 </file>
@@ -666,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -703,7 +721,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -712,6 +729,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1017,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="B251" activeCellId="2" sqref="C251 B251 B251"/>
+    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="A257" sqref="A257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1052,7 @@
     <col min="1" max="1" width="23.5703125" style="12" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1063,11 +1089,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>774</v>
+        <v>782</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>68.13333333333334</v>
+        <v>68.966666666666669</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1190,7 +1216,7 @@
       <c r="C14" s="9">
         <v>0</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="21" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2381,7 +2407,7 @@
       <c r="C122" s="8">
         <v>0</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="21" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2615,7 +2641,7 @@
       <c r="C143" s="1">
         <v>32</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="21" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2783,7 +2809,7 @@
       <c r="C158" s="8">
         <v>0</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="21" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2962,7 +2988,7 @@
       <c r="C174" s="8">
         <v>0</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="21" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3031,7 +3057,7 @@
       <c r="C180" s="8">
         <v>0</v>
       </c>
-      <c r="D180" s="20" t="s">
+      <c r="D180" s="19" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3045,7 +3071,7 @@
       <c r="C181" s="8">
         <v>0</v>
       </c>
-      <c r="D181" s="20"/>
+      <c r="D181" s="19"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="14">
@@ -3057,7 +3083,7 @@
       <c r="C182" s="8">
         <v>0</v>
       </c>
-      <c r="D182" s="20"/>
+      <c r="D182" s="19"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="10">
@@ -3201,7 +3227,7 @@
       <c r="C195" s="1">
         <v>0</v>
       </c>
-      <c r="D195" s="16" t="s">
+      <c r="D195" s="22" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3248,7 +3274,7 @@
       <c r="C199" s="1">
         <v>0</v>
       </c>
-      <c r="D199" s="16" t="s">
+      <c r="D199" s="22" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3328,7 +3354,7 @@
       <c r="C206" s="1">
         <v>29</v>
       </c>
-      <c r="D206" s="16" t="s">
+      <c r="D206" s="22" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3342,7 +3368,7 @@
       <c r="C207" s="1">
         <v>0</v>
       </c>
-      <c r="D207" s="16" t="s">
+      <c r="D207" s="22" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3402,182 +3428,182 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="17">
+      <c r="A213" s="16">
         <v>41529</v>
       </c>
-      <c r="B213" s="18"/>
-      <c r="C213" s="18"/>
-      <c r="D213" s="20" t="s">
+      <c r="B213" s="17"/>
+      <c r="C213" s="17"/>
+      <c r="D213" s="19" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="17">
+      <c r="A214" s="16">
         <v>41559</v>
       </c>
-      <c r="B214" s="18"/>
-      <c r="C214" s="18"/>
-      <c r="D214" s="20"/>
+      <c r="B214" s="17"/>
+      <c r="C214" s="17"/>
+      <c r="D214" s="19"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="17">
+      <c r="A215" s="16">
         <v>41590</v>
       </c>
-      <c r="B215" s="18"/>
-      <c r="C215" s="18"/>
-      <c r="D215" s="20"/>
+      <c r="B215" s="17"/>
+      <c r="C215" s="17"/>
+      <c r="D215" s="19"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="17">
+      <c r="A216" s="16">
         <v>41620</v>
       </c>
-      <c r="B216" s="18"/>
-      <c r="C216" s="18"/>
-      <c r="D216" s="20"/>
+      <c r="B216" s="17"/>
+      <c r="C216" s="17"/>
+      <c r="D216" s="19"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="17" t="s">
+      <c r="A217" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B217" s="18"/>
-      <c r="C217" s="18"/>
-      <c r="D217" s="20"/>
+      <c r="B217" s="17"/>
+      <c r="C217" s="17"/>
+      <c r="D217" s="19"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="17" t="s">
+      <c r="A218" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B218" s="18"/>
-      <c r="C218" s="18"/>
-      <c r="D218" s="20"/>
+      <c r="B218" s="17"/>
+      <c r="C218" s="17"/>
+      <c r="D218" s="19"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="17" t="s">
+      <c r="A219" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B219" s="18"/>
-      <c r="C219" s="18"/>
-      <c r="D219" s="20"/>
+      <c r="B219" s="17"/>
+      <c r="C219" s="17"/>
+      <c r="D219" s="19"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" s="17" t="s">
+      <c r="A220" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="B220" s="18"/>
-      <c r="C220" s="18"/>
-      <c r="D220" s="20"/>
+      <c r="B220" s="17"/>
+      <c r="C220" s="17"/>
+      <c r="D220" s="19"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="17" t="s">
+      <c r="A221" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="B221" s="18"/>
-      <c r="C221" s="18"/>
-      <c r="D221" s="20"/>
+      <c r="B221" s="17"/>
+      <c r="C221" s="17"/>
+      <c r="D221" s="19"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="17" t="s">
+      <c r="A222" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="B222" s="18"/>
-      <c r="C222" s="18"/>
-      <c r="D222" s="20"/>
+      <c r="B222" s="17"/>
+      <c r="C222" s="17"/>
+      <c r="D222" s="19"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="17" t="s">
+      <c r="A223" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="B223" s="18"/>
-      <c r="C223" s="18"/>
-      <c r="D223" s="20"/>
+      <c r="B223" s="17"/>
+      <c r="C223" s="17"/>
+      <c r="D223" s="19"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="17" t="s">
+      <c r="A224" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B224" s="18"/>
-      <c r="C224" s="18"/>
-      <c r="D224" s="20"/>
+      <c r="B224" s="17"/>
+      <c r="C224" s="17"/>
+      <c r="D224" s="19"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="17" t="s">
+      <c r="A225" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="B225" s="18"/>
-      <c r="C225" s="18"/>
-      <c r="D225" s="20"/>
+      <c r="B225" s="17"/>
+      <c r="C225" s="17"/>
+      <c r="D225" s="19"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="17" t="s">
+      <c r="A226" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="B226" s="18"/>
-      <c r="C226" s="18"/>
-      <c r="D226" s="20"/>
+      <c r="B226" s="17"/>
+      <c r="C226" s="17"/>
+      <c r="D226" s="19"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="17" t="s">
+      <c r="A227" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B227" s="18"/>
-      <c r="C227" s="18"/>
-      <c r="D227" s="20"/>
+      <c r="B227" s="17"/>
+      <c r="C227" s="17"/>
+      <c r="D227" s="19"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="17" t="s">
+      <c r="A228" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="B228" s="18"/>
-      <c r="C228" s="18"/>
-      <c r="D228" s="20"/>
+      <c r="B228" s="17"/>
+      <c r="C228" s="17"/>
+      <c r="D228" s="19"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="19" t="s">
+      <c r="A229" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="B229" s="18"/>
-      <c r="C229" s="18"/>
-      <c r="D229" s="20"/>
+      <c r="B229" s="17"/>
+      <c r="C229" s="17"/>
+      <c r="D229" s="19"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="19" t="s">
+      <c r="A230" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B230" s="18"/>
-      <c r="C230" s="18"/>
-      <c r="D230" s="20"/>
+      <c r="B230" s="17"/>
+      <c r="C230" s="17"/>
+      <c r="D230" s="19"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="19" t="s">
+      <c r="A231" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="B231" s="18"/>
-      <c r="C231" s="18"/>
-      <c r="D231" s="20"/>
+      <c r="B231" s="17"/>
+      <c r="C231" s="17"/>
+      <c r="D231" s="19"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="19" t="s">
+      <c r="A232" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="B232" s="18"/>
-      <c r="C232" s="18"/>
-      <c r="D232" s="20"/>
+      <c r="B232" s="17"/>
+      <c r="C232" s="17"/>
+      <c r="D232" s="19"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="19" t="s">
+      <c r="A233" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="B233" s="18"/>
-      <c r="C233" s="18"/>
-      <c r="D233" s="20"/>
+      <c r="B233" s="17"/>
+      <c r="C233" s="17"/>
+      <c r="D233" s="19"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="19" t="s">
+      <c r="A234" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="B234" s="18"/>
-      <c r="C234" s="18"/>
-      <c r="D234" s="20"/>
+      <c r="B234" s="17"/>
+      <c r="C234" s="17"/>
+      <c r="D234" s="19"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="11" t="s">
@@ -3645,7 +3671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="10">
         <v>41426</v>
       </c>
@@ -3656,7 +3682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="10">
         <v>41456</v>
       </c>
@@ -3667,7 +3693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="10">
         <v>41487</v>
       </c>
@@ -3678,7 +3704,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="10">
         <v>41518</v>
       </c>
@@ -3689,7 +3715,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="10">
         <v>41548</v>
       </c>
@@ -3700,7 +3726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="10">
         <v>41579</v>
       </c>
@@ -3711,7 +3737,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="10">
         <v>41609</v>
       </c>
@@ -3722,7 +3748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="11" t="s">
         <v>163</v>
       </c>
@@ -3733,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="11" t="s">
         <v>164</v>
       </c>
@@ -3744,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="11" t="s">
         <v>165</v>
       </c>
@@ -3755,7 +3781,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="11" t="s">
         <v>166</v>
       </c>
@@ -3766,30 +3792,65 @@
         <v>30</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" s="11"/>
-      <c r="B252" s="1"/>
-      <c r="C252" s="1"/>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" s="11"/>
-      <c r="B253" s="1"/>
-      <c r="C253" s="1"/>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254" s="11"/>
-      <c r="B254" s="1"/>
-      <c r="C254" s="1"/>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A255" s="11"/>
-      <c r="B255" s="1"/>
-      <c r="C255" s="1"/>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A256" s="11"/>
-      <c r="B256" s="1"/>
-      <c r="C256" s="1"/>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B252" s="1">
+        <v>5</v>
+      </c>
+      <c r="C252" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B253" s="8">
+        <v>0</v>
+      </c>
+      <c r="C253" s="8">
+        <v>0</v>
+      </c>
+      <c r="D253" s="20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B254" s="8">
+        <v>0</v>
+      </c>
+      <c r="C254" s="8">
+        <v>0</v>
+      </c>
+      <c r="D254" s="20"/>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B255" s="8">
+        <v>0</v>
+      </c>
+      <c r="C255" s="8">
+        <v>0</v>
+      </c>
+      <c r="D255" s="20"/>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B256" s="1">
+        <v>3</v>
+      </c>
+      <c r="C256" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="11"/>
@@ -3837,9 +3898,10 @@
       <c r="C265" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D180:D182"/>
     <mergeCell ref="D213:D234"/>
+    <mergeCell ref="D253:D255"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
time update and string matching counter
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
   <si>
     <t>Date</t>
   </si>
@@ -547,6 +547,9 @@
   </si>
   <si>
     <t>25/1/2014</t>
+  </si>
+  <si>
+    <t>26/1/2014</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1059,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
-      <selection activeCell="G279" sqref="G279"/>
+      <selection activeCell="C262" sqref="C262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1104,7 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>802</v>
+        <v>807</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
@@ -3909,9 +3912,15 @@
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A261" s="11"/>
-      <c r="B261" s="1"/>
-      <c r="C261" s="1"/>
+      <c r="A261" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B261" s="1">
+        <v>5</v>
+      </c>
+      <c r="C261" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="11"/>

</xml_diff>

<commit_message>
time update, damminda meeting recording
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="180">
   <si>
     <t>Date</t>
   </si>
@@ -553,6 +553,9 @@
   </si>
   <si>
     <t>27/1/2014</t>
+  </si>
+  <si>
+    <t>28/1/2013</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1065,7 @@
   <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
-      <selection activeCell="A262" sqref="A262"/>
+      <selection activeCell="B262" sqref="B262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,11 +1110,11 @@
       </c>
       <c r="G3">
         <f>SUM(B2:B265)</f>
-        <v>811</v>
+        <v>826</v>
       </c>
       <c r="H3">
         <f>SUM(C2:C265)/60</f>
-        <v>70.966666666666669</v>
+        <v>71.716666666666669</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3930,16 +3933,22 @@
         <v>178</v>
       </c>
       <c r="B262" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C262" s="1">
         <v>45</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263" s="11"/>
-      <c r="B263" s="1"/>
-      <c r="C263" s="1"/>
+      <c r="A263" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B263" s="1">
+        <v>13</v>
+      </c>
+      <c r="C263" s="1">
+        <v>45</v>
+      </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="11"/>

</xml_diff>

<commit_message>
time update and code modification
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="193">
   <si>
     <t>Date</t>
   </si>
@@ -589,6 +589,12 @@
   </si>
   <si>
     <t>20/2/2014</t>
+  </si>
+  <si>
+    <t>21/2/2014</t>
+  </si>
+  <si>
+    <t>22/2/2014</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1104,7 @@
   <dimension ref="A1:H415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="E283" sqref="E283"/>
+      <selection activeCell="B294" sqref="B294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4237,12 +4243,20 @@
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A287" s="11"/>
-      <c r="B287" s="1"/>
-      <c r="C287" s="1"/>
+      <c r="A287" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B287" s="1">
+        <v>8</v>
+      </c>
+      <c r="C287" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" s="11"/>
+      <c r="A288" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="B288" s="1"/>
       <c r="C288" s="1"/>
     </row>

</xml_diff>

<commit_message>
time update and efficient input
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -1104,7 +1104,7 @@
   <dimension ref="A1:H415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="C289" sqref="C289"/>
+      <selection activeCell="C292" sqref="C292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4258,10 +4258,10 @@
         <v>192</v>
       </c>
       <c r="B288" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C288" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
time update + efficient code
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -1122,7 +1122,7 @@
   <dimension ref="A1:H415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="B293" sqref="B293"/>
+      <selection activeCell="C296" sqref="C296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4341,8 +4341,12 @@
       <c r="A294" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="B294" s="1"/>
-      <c r="C294" s="1"/>
+      <c r="B294" s="1">
+        <v>1</v>
+      </c>
+      <c r="C294" s="1">
+        <v>35</v>
+      </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="11"/>

</xml_diff>

<commit_message>
time update results add
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -1122,7 +1122,7 @@
   <dimension ref="A1:H415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="C297" sqref="C297"/>
+      <selection activeCell="A300" sqref="A300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4364,16 +4364,22 @@
         <v>41673</v>
       </c>
       <c r="B296" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C296" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A297" s="11"/>
-      <c r="B297" s="1"/>
-      <c r="C297" s="1"/>
+      <c r="A297" s="10">
+        <v>41701</v>
+      </c>
+      <c r="B297" s="1">
+        <v>3</v>
+      </c>
+      <c r="C297" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="11"/>

</xml_diff>

<commit_message>
time update/ updates of code
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -4382,14 +4382,26 @@
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A298" s="11"/>
-      <c r="B298" s="1"/>
-      <c r="C298" s="1"/>
+      <c r="A298" s="10">
+        <v>41732</v>
+      </c>
+      <c r="B298" s="1">
+        <v>1</v>
+      </c>
+      <c r="C298" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A299" s="11"/>
-      <c r="B299" s="1"/>
-      <c r="C299" s="1"/>
+      <c r="A299" s="10">
+        <v>41762</v>
+      </c>
+      <c r="B299" s="1">
+        <v>6</v>
+      </c>
+      <c r="C299" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="11"/>

</xml_diff>

<commit_message>
time update and bug fixes
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -1122,7 +1122,7 @@
   <dimension ref="A1:H415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="C302" sqref="C302"/>
+      <selection activeCell="E301" sqref="E301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4419,10 +4419,10 @@
         <v>41823</v>
       </c>
       <c r="B301" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C301" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
time update and modification of code
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="A328" sqref="A328"/>
+    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="C336" sqref="C336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4780,39 +4780,81 @@
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A329" s="11"/>
-      <c r="B329" s="1"/>
-      <c r="C329" s="1"/>
+      <c r="A329" s="10">
+        <v>41733</v>
+      </c>
+      <c r="B329" s="1">
+        <v>6</v>
+      </c>
+      <c r="C329" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A330" s="11"/>
-      <c r="B330" s="1"/>
-      <c r="C330" s="1"/>
+      <c r="A330" s="10">
+        <v>41763</v>
+      </c>
+      <c r="B330" s="1">
+        <v>8</v>
+      </c>
+      <c r="C330" s="1">
+        <v>42</v>
+      </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A331" s="11"/>
-      <c r="B331" s="1"/>
-      <c r="C331" s="1"/>
+      <c r="A331" s="10">
+        <v>41794</v>
+      </c>
+      <c r="B331" s="1">
+        <v>0</v>
+      </c>
+      <c r="C331" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A332" s="11"/>
-      <c r="B332" s="1"/>
-      <c r="C332" s="1"/>
+      <c r="A332" s="10">
+        <v>41824</v>
+      </c>
+      <c r="B332" s="1">
+        <v>0</v>
+      </c>
+      <c r="C332" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A333" s="11"/>
-      <c r="B333" s="1"/>
-      <c r="C333" s="1"/>
+      <c r="A333" s="10">
+        <v>41855</v>
+      </c>
+      <c r="B333" s="1">
+        <v>3</v>
+      </c>
+      <c r="C333" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A334" s="11"/>
-      <c r="B334" s="1"/>
-      <c r="C334" s="1"/>
+      <c r="A334" s="10">
+        <v>41886</v>
+      </c>
+      <c r="B334" s="1">
+        <v>4</v>
+      </c>
+      <c r="C334" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A335" s="11"/>
-      <c r="B335" s="1"/>
-      <c r="C335" s="1"/>
+      <c r="A335" s="10">
+        <v>41916</v>
+      </c>
+      <c r="B335" s="1">
+        <v>5</v>
+      </c>
+      <c r="C335" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="11"/>

</xml_diff>

<commit_message>
time update /result update
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" workbookViewId="0">
-      <selection activeCell="D348" sqref="D348"/>
+    <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
+      <selection activeCell="F368" sqref="F368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4131,10 +4131,10 @@
       <c r="A267" s="10">
         <v>41641</v>
       </c>
-      <c r="B267" s="1">
-        <v>0</v>
-      </c>
-      <c r="C267" s="1">
+      <c r="B267" s="9">
+        <v>0</v>
+      </c>
+      <c r="C267" s="9">
         <v>0</v>
       </c>
     </row>
@@ -4142,10 +4142,10 @@
       <c r="A268" s="10">
         <v>41672</v>
       </c>
-      <c r="B268" s="1">
-        <v>0</v>
-      </c>
-      <c r="C268" s="1">
+      <c r="B268" s="9">
+        <v>0</v>
+      </c>
+      <c r="C268" s="9">
         <v>0</v>
       </c>
     </row>
@@ -4208,10 +4208,10 @@
       <c r="A274" s="10">
         <v>41853</v>
       </c>
-      <c r="B274" s="1">
-        <v>0</v>
-      </c>
-      <c r="C274" s="1">
+      <c r="B274" s="9">
+        <v>0</v>
+      </c>
+      <c r="C274" s="9">
         <v>0</v>
       </c>
     </row>
@@ -4549,10 +4549,10 @@
       <c r="A305" s="10">
         <v>41946</v>
       </c>
-      <c r="B305" s="1">
-        <v>0</v>
-      </c>
-      <c r="C305" s="1">
+      <c r="B305" s="9">
+        <v>0</v>
+      </c>
+      <c r="C305" s="9">
         <v>0</v>
       </c>
     </row>
@@ -4681,10 +4681,10 @@
       <c r="A317" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B317" s="1">
-        <v>0</v>
-      </c>
-      <c r="C317" s="1">
+      <c r="B317" s="9">
+        <v>0</v>
+      </c>
+      <c r="C317" s="9">
         <v>0</v>
       </c>
     </row>
@@ -4978,10 +4978,10 @@
       <c r="A344" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="B344" s="1">
-        <v>0</v>
-      </c>
-      <c r="C344" s="1">
+      <c r="B344" s="9">
+        <v>0</v>
+      </c>
+      <c r="C344" s="9">
         <v>0</v>
       </c>
     </row>
@@ -5012,7 +5012,7 @@
         <v>227</v>
       </c>
       <c r="B347" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C347" s="1">
         <v>47</v>

</xml_diff>

<commit_message>
time update and data update
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="230">
   <si>
     <t>Date</t>
   </si>
@@ -703,6 +703,9 @@
   </si>
   <si>
     <t>23/4/2014</t>
+  </si>
+  <si>
+    <t>24/4/2014</t>
   </si>
 </sst>
 </file>
@@ -1212,7 +1215,7 @@
   <dimension ref="A1:H415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
-      <selection activeCell="D350" sqref="D350"/>
+      <selection activeCell="C350" sqref="C350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5033,9 +5036,15 @@
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A349" s="11"/>
-      <c r="B349" s="1"/>
-      <c r="C349" s="1"/>
+      <c r="A349" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B349" s="1">
+        <v>5</v>
+      </c>
+      <c r="C349" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="11"/>

</xml_diff>

<commit_message>
time update, results and file update
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="232">
   <si>
     <t>Date</t>
   </si>
@@ -709,6 +709,9 @@
   </si>
   <si>
     <t>25/4/2014</t>
+  </si>
+  <si>
+    <t>26/4/2014</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1221,7 @@
   <dimension ref="A1:H415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
-      <selection activeCell="C351" sqref="C351"/>
+      <selection activeCell="C352" sqref="C352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5061,9 +5064,15 @@
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A351" s="11"/>
-      <c r="B351" s="1"/>
-      <c r="C351" s="1"/>
+      <c r="A351" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B351" s="1">
+        <v>6</v>
+      </c>
+      <c r="C351" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="11"/>

</xml_diff>

<commit_message>
time update and new data files
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="238">
   <si>
     <t>Date</t>
   </si>
@@ -724,6 +724,12 @@
   </si>
   <si>
     <t>30/4/2014</t>
+  </si>
+  <si>
+    <t>Orbing</t>
+  </si>
+  <si>
+    <t>Kasun Case</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1239,7 @@
   <dimension ref="A1:H415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
-      <selection activeCell="C356" sqref="C356"/>
+      <selection activeCell="C360" sqref="C360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5097,7 +5103,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" s="11" t="s">
         <v>233</v>
       </c>
@@ -5108,7 +5114,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" s="11" t="s">
         <v>234</v>
       </c>
@@ -5119,7 +5125,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" s="11" t="s">
         <v>235</v>
       </c>
@@ -5130,67 +5136,97 @@
         <v>16</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A356" s="11"/>
-      <c r="B356" s="1"/>
-      <c r="C356" s="1"/>
-    </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A357" s="11"/>
-      <c r="B357" s="1"/>
-      <c r="C357" s="1"/>
-    </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A358" s="11"/>
-      <c r="B358" s="1"/>
-      <c r="C358" s="1"/>
-    </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A359" s="11"/>
-      <c r="B359" s="1"/>
-      <c r="C359" s="1"/>
-    </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356" s="10">
+        <v>41644</v>
+      </c>
+      <c r="B356" s="1">
+        <v>2</v>
+      </c>
+      <c r="C356" s="1">
+        <v>5</v>
+      </c>
+      <c r="D356" s="19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A357" s="10">
+        <v>41675</v>
+      </c>
+      <c r="B357" s="1">
+        <v>5</v>
+      </c>
+      <c r="C357" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A358" s="10">
+        <v>41703</v>
+      </c>
+      <c r="B358" s="1">
+        <v>2</v>
+      </c>
+      <c r="C358" s="1">
+        <v>0</v>
+      </c>
+      <c r="D358" s="19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A359" s="10">
+        <v>41734</v>
+      </c>
+      <c r="B359" s="1">
+        <v>4</v>
+      </c>
+      <c r="C359" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" s="11"/>
       <c r="B360" s="1"/>
       <c r="C360" s="1"/>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" s="11"/>
       <c r="B361" s="1"/>
       <c r="C361" s="1"/>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" s="11"/>
       <c r="B362" s="1"/>
       <c r="C362" s="1"/>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" s="11"/>
       <c r="B363" s="1"/>
       <c r="C363" s="1"/>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" s="11"/>
       <c r="B364" s="1"/>
       <c r="C364" s="1"/>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" s="11"/>
       <c r="B365" s="1"/>
       <c r="C365" s="1"/>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" s="11"/>
       <c r="B366" s="1"/>
       <c r="C366" s="1"/>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" s="11"/>
       <c r="B367" s="1"/>
       <c r="C367" s="1"/>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" s="11"/>
       <c r="B368" s="1"/>
       <c r="C368" s="1"/>

</xml_diff>

<commit_message>
time update/ bug fixes to SOM
</commit_message>
<xml_diff>
--- a/Time Keeping/Work Hours.xlsx
+++ b/Time Keeping/Work Hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="247">
   <si>
     <t>Date</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t>20/5/2014</t>
+  </si>
+  <si>
+    <t>21/5/2014</t>
   </si>
 </sst>
 </file>
@@ -1263,7 +1266,7 @@
   <dimension ref="A1:H415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
-      <selection activeCell="B375" sqref="B375"/>
+      <selection activeCell="C377" sqref="C377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5387,9 +5390,15 @@
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A376" s="11"/>
-      <c r="B376" s="1"/>
-      <c r="C376" s="1"/>
+      <c r="A376" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B376" s="1">
+        <v>7</v>
+      </c>
+      <c r="C376" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="11"/>

</xml_diff>